<commit_message>
fix: finalização dos ajustes do storage manager
</commit_message>
<xml_diff>
--- a/arquivos/coleta_dados_spotify.xlsx
+++ b/arquivos/coleta_dados_spotify.xlsx
@@ -1699,14 +1699,599 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>trackUri</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>trackTitle</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>roleTitle</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>artist_uri</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>artist_name</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>artist_image_uri</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>artist_subroles</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>artist_weight</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>artist_external_url</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>artist_creator_uri</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>spotify:track:1w7cgGZR86yWz1pA2puVJD</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>HEATED</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Performers</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>spotify:artist:6vWDO969PvNqNYHIOW5v0m</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Beyoncé</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>https://i.scdn.co/image/ab677762000078e645c984e8c82f9ce15ebf1f51</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>['main artist']</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>0.8999000191688538</v>
+      </c>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>spotify:track:1w7cgGZR86yWz1pA2puVJD</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>HEATED</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Writers</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Brittany "@Chi_Coney" Coney</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>https://artists.spotify.com/songwriter/1uYXu9L0vzo1lcJk7SjgCT</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>spotify:songwriter:1uYXu9L0vzo1lcJk7SjgCT</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>spotify:track:1w7cgGZR86yWz1pA2puVJD</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>HEATED</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Writers</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Denisia "Blu June" Andrews</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>https://artists.spotify.com/songwriter/6usZxRd8e7TQwcksnohR1U</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>spotify:songwriter:6usZxRd8e7TQwcksnohR1U</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>spotify:track:1w7cgGZR86yWz1pA2puVJD</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>HEATED</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Writers</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>A. Graham</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>spotify:track:1w7cgGZR86yWz1pA2puVJD</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>HEATED</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Producers</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>spotify:artist:2pSxft78wxISNLTbjFThTk</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Cadenza</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>https://i.scdn.co/image/ab677762000078e6afc079cda32d54850e82c385</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>['producer']</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>0.548799991607666</v>
+      </c>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>spotify:track:1w7cgGZR86yWz1pA2puVJD</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>HEATED</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Producers</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>spotify:artist:6PIl48ctj6HDmqVM2uIikd</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Kelman Duran</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>https://i.scdn.co/image/ab677762000078e645c984e8c82f9ce15ebf1f51</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>['producer']</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>0.5483999848365784</v>
+      </c>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>spotify:track:1w7cgGZR86yWz1pA2puVJD</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>HEATED</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Producers</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>spotify:artist:7rzPhcWW1k8njDS5r2xbWe</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Jahaan Sweet</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>https://i.scdn.co/image/ab677762000078e6afc079cda32d54850e82c385</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>['producer']</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
+        <v>0.5480999946594238</v>
+      </c>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>spotify:track:1w7cgGZR86yWz1pA2puVJD</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>HEATED</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Producers</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>spotify:artist:2TRy6nJhEnznYDL0AtYJAI</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Stuart White</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>https://i.scdn.co/image/ab677762000078e6d2b377637d9f6ed34f1652e2</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>['producer']</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>0.5473999977111816</v>
+      </c>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>spotify:track:1w7cgGZR86yWz1pA2puVJD</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>HEATED</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Producers</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>spotify:artist:0NPWbgGDaiX1yZaN0nzhqn</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Neenyo</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>https://i.scdn.co/image/ab677762000078e6d2b377637d9f6ed34f1652e2</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>['producer']</t>
+        </is>
+      </c>
+      <c r="I10" t="n">
+        <v>0.5472000241279602</v>
+      </c>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>spotify:track:1w7cgGZR86yWz1pA2puVJD</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>HEATED</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Producers</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>spotify:artist:6T9dsSIQ31Sk8x24lwfTG4</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Sevn Thomas</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>https://i.scdn.co/image/ab677762000078e6d2b377637d9f6ed34f1652e2</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>['producer']</t>
+        </is>
+      </c>
+      <c r="I11" t="n">
+        <v>0.5468999743461609</v>
+      </c>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>spotify:track:1w7cgGZR86yWz1pA2puVJD</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>HEATED</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Producers</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>spotify:artist:2RQnTQM6OQd8dTUDF7UsT7</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Boi-1da</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>https://i.scdn.co/image/ab677762000078e6aae517f57fa4e9833b4bce9c</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>['producer']</t>
+        </is>
+      </c>
+      <c r="I12" t="n">
+        <v>0.5468000173568726</v>
+      </c>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>spotify:track:1w7cgGZR86yWz1pA2puVJD</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>HEATED</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Producers</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>spotify:artist:3FdxqLD6H5pfO0C0kd9YYt</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Harry Edwards</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>https://i.scdn.co/image/ab677762000078e645c984e8c82f9ce15ebf1f51</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>['producer']</t>
+        </is>
+      </c>
+      <c r="I13" t="n">
+        <v>0.5461000204086304</v>
+      </c>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
feat: ajustes no código da main e remoção de prints
</commit_message>
<xml_diff>
--- a/arquivos/coleta_dados_spotify.xlsx
+++ b/arquivos/coleta_dados_spotify.xlsx
@@ -543,7 +543,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -671,6 +671,2995 @@
       <c r="M2" t="inlineStr">
         <is>
           <t>spotify:album:6FJxoadUE4JNVwWHghBwnb</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/7kUuNU2LRmr9XbwLHXU9UZ'}</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/7kUuNU2LRmr9XbwLHXU9UZ</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>7kUuNU2LRmr9XbwLHXU9UZ</t>
+        </is>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>The Lion King: The Gift [Deluxe Edition]</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>2020-07-31</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K3" t="n">
+        <v>17</v>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>spotify:album:7kUuNU2LRmr9XbwLHXU9UZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/552zi1M53PQAX5OH4FIdTx'}</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/552zi1M53PQAX5OH4FIdTx</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>552zi1M53PQAX5OH4FIdTx</t>
+        </is>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>The Lion King: The Gift</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>2019-07-19</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K4" t="n">
+        <v>27</v>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>spotify:album:552zi1M53PQAX5OH4FIdTx</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/35S1JCj5paIfElT2GODl6x'}</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/35S1JCj5paIfElT2GODl6x</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>35S1JCj5paIfElT2GODl6x</t>
+        </is>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>HOMECOMING: THE LIVE ALBUM</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>2019-04-17</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K5" t="n">
+        <v>40</v>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>spotify:album:35S1JCj5paIfElT2GODl6x</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/7dK54iZuOxXFarGhXwEXfF'}</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/7dK54iZuOxXFarGhXwEXfF</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>7dK54iZuOxXFarGhXwEXfF</t>
+        </is>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Lemonade</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>2016-04-23</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K6" t="n">
+        <v>13</v>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>spotify:album:7dK54iZuOxXFarGhXwEXfF</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/2UJwKSBUz6rtW4QLK74kQu'}</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/2UJwKSBUz6rtW4QLK74kQu</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2UJwKSBUz6rtW4QLK74kQu</t>
+        </is>
+      </c>
+      <c r="G7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>BEYONCÉ [Platinum Edition]</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>2014-11-24</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K7" t="n">
+        <v>20</v>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>spotify:album:2UJwKSBUz6rtW4QLK74kQu</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/1gIC63gC3B7o7FfpPACZQJ'}</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/1gIC63gC3B7o7FfpPACZQJ</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>1gIC63gC3B7o7FfpPACZQJ</t>
+        </is>
+      </c>
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>2011-06-24</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K8" t="n">
+        <v>14</v>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>spotify:album:1gIC63gC3B7o7FfpPACZQJ</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/5O7PYNgE3VLWrvB80fIaDZ'}</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/5O7PYNgE3VLWrvB80fIaDZ</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>5O7PYNgE3VLWrvB80fIaDZ</t>
+        </is>
+      </c>
+      <c r="G9" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>I Am...World Tour</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>2010-11-26</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K9" t="n">
+        <v>25</v>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>spotify:album:5O7PYNgE3VLWrvB80fIaDZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/23Y5wdyP5byMFktZf8AcWU'}</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/23Y5wdyP5byMFktZf8AcWU</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>23Y5wdyP5byMFktZf8AcWU</t>
+        </is>
+      </c>
+      <c r="G10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>I AM...SASHA FIERCE</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>2008-11-14</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K10" t="n">
+        <v>16</v>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>spotify:album:23Y5wdyP5byMFktZf8AcWU</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/46BXsx30qaCaAyyGtWyx7e'}</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/46BXsx30qaCaAyyGtWyx7e</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>46BXsx30qaCaAyyGtWyx7e</t>
+        </is>
+      </c>
+      <c r="G11" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>The Beyonce Experience Live Audio</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>2007-11-19</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K11" t="n">
+        <v>21</v>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>spotify:album:46BXsx30qaCaAyyGtWyx7e</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/0Zd10MKN5j9KwUST0TdBBB'}</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/0Zd10MKN5j9KwUST0TdBBB</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>0Zd10MKN5j9KwUST0TdBBB</t>
+        </is>
+      </c>
+      <c r="G12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>B'Day Deluxe Edition</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>2007-05-29</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K12" t="n">
+        <v>23</v>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>spotify:album:0Zd10MKN5j9KwUST0TdBBB</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/77eZ5eMEh3U0KWricrbevO'}</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/77eZ5eMEh3U0KWricrbevO</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>77eZ5eMEh3U0KWricrbevO</t>
+        </is>
+      </c>
+      <c r="G13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>B'Day</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>2006-09-04</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K13" t="n">
+        <v>11</v>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>spotify:album:77eZ5eMEh3U0KWricrbevO</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/06v9eHnqhMK2tbM2Iz3p0Y'}</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/06v9eHnqhMK2tbM2Iz3p0Y</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>06v9eHnqhMK2tbM2Iz3p0Y</t>
+        </is>
+      </c>
+      <c r="G14" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Dangerously In Love</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>2003-03-10</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K14" t="n">
+        <v>16</v>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>spotify:album:06v9eHnqhMK2tbM2Iz3p0Y</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/0219TxSZyWhfo1DgafkjX2'}</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/0219TxSZyWhfo1DgafkjX2</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>0219TxSZyWhfo1DgafkjX2</t>
+        </is>
+      </c>
+      <c r="G15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>DELRESTO (ECHOES)</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>2023-07-26</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K15" t="n">
+        <v>1</v>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>spotify:album:0219TxSZyWhfo1DgafkjX2</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/2x4aShbWkdZ1h8sfO23yZN'}</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/2x4aShbWkdZ1h8sfO23yZN</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2x4aShbWkdZ1h8sfO23yZN</t>
+        </is>
+      </c>
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>AMERICA HAS A PROBLEM (feat. Kendrick Lamar)</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>2023-05-19</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K16" t="n">
+        <v>1</v>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>spotify:album:2x4aShbWkdZ1h8sfO23yZN</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/7BJjZgzGzpll0t8CEzjILs'}</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/7BJjZgzGzpll0t8CEzjILs</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>7BJjZgzGzpll0t8CEzjILs</t>
+        </is>
+      </c>
+      <c r="G17" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>CUFF IT</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>2023-02-08</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K17" t="n">
+        <v>3</v>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>spotify:album:7BJjZgzGzpll0t8CEzjILs</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/43geArd3U23pTVjqzTSnkI'}</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/43geArd3U23pTVjqzTSnkI</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>43geArd3U23pTVjqzTSnkI</t>
+        </is>
+      </c>
+      <c r="G18" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>BREAK MY SOUL REMIXES</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>2022-07-26</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K18" t="n">
+        <v>4</v>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>spotify:album:43geArd3U23pTVjqzTSnkI</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/4xm2wzhAU05Y4dEdj1BO5J'}</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/4xm2wzhAU05Y4dEdj1BO5J</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>4xm2wzhAU05Y4dEdj1BO5J</t>
+        </is>
+      </c>
+      <c r="G19" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>BREAK MY SOUL (THE QUEENS REMIX)</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>2022-07-26</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K19" t="n">
+        <v>1</v>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>spotify:album:4xm2wzhAU05Y4dEdj1BO5J</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/5HVPAGU1Qx7LpZtnr1i8mK'}</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/5HVPAGU1Qx7LpZtnr1i8mK</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>5HVPAGU1Qx7LpZtnr1i8mK</t>
+        </is>
+      </c>
+      <c r="G20" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>BREAK MY SOUL</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>2022-07-22</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K20" t="n">
+        <v>3</v>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>spotify:album:5HVPAGU1Qx7LpZtnr1i8mK</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/5a73HUmrKIebjmafM1QuFS'}</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/5a73HUmrKIebjmafM1QuFS</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>5a73HUmrKIebjmafM1QuFS</t>
+        </is>
+      </c>
+      <c r="G21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Be Alive (Original Song from the Motion Picture "King Richard")</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>2021-11-12</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K21" t="n">
+        <v>1</v>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>spotify:album:5a73HUmrKIebjmafM1QuFS</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/3MJxH055n52Rbm8RLlpJcN'}</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/3MJxH055n52Rbm8RLlpJcN</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>3MJxH055n52Rbm8RLlpJcN</t>
+        </is>
+      </c>
+      <c r="G22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>BLACK PARADE</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>2020-06-19</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K22" t="n">
+        <v>1</v>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>spotify:album:3MJxH055n52Rbm8RLlpJcN</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/6M4VOF1ExBRii1x20Pk0GR'}</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/6M4VOF1ExBRii1x20Pk0GR</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>6M4VOF1ExBRii1x20Pk0GR</t>
+        </is>
+      </c>
+      <c r="G23" t="b">
+        <v>1</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Savage Remix (feat. Beyoncé)</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>2020-04-29</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K23" t="n">
+        <v>1</v>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>spotify:album:6M4VOF1ExBRii1x20Pk0GR</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/6W0hMM8vjhNhDOjfiORZE4'}</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/6W0hMM8vjhNhDOjfiORZE4</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>6W0hMM8vjhNhDOjfiORZE4</t>
+        </is>
+      </c>
+      <c r="G24" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>SPIRIT (From Disney's "The Lion King")</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>2019-07-10</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K24" t="n">
+        <v>1</v>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>spotify:album:6W0hMM8vjhNhDOjfiORZE4</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/5PWAVs0wbPUh0NNPM9xxNn'}</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/5PWAVs0wbPUh0NNPM9xxNn</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>5PWAVs0wbPUh0NNPM9xxNn</t>
+        </is>
+      </c>
+      <c r="G25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Survivor / Moment Musical No. 4 (From 6 Moments Musicaux, Op. 16)</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>2018-11-30</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K25" t="n">
+        <v>1</v>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>spotify:album:5PWAVs0wbPUh0NNPM9xxNn</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/52kvZcbEDm0v2kWZQXjuuA'}</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/52kvZcbEDm0v2kWZQXjuuA</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>52kvZcbEDm0v2kWZQXjuuA</t>
+        </is>
+      </c>
+      <c r="G26" t="b">
+        <v>1</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Perfect Duet (Ed Sheeran &amp; Beyoncé)</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>2017-11-30</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K26" t="n">
+        <v>1</v>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>spotify:album:52kvZcbEDm0v2kWZQXjuuA</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/7vmngE1EExuJ0wpdRescsX'}</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/7vmngE1EExuJ0wpdRescsX</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>7vmngE1EExuJ0wpdRescsX</t>
+        </is>
+      </c>
+      <c r="G27" t="b">
+        <v>1</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Daddy Lessons</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>2016-11-20</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K27" t="n">
+        <v>1</v>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>spotify:album:7vmngE1EExuJ0wpdRescsX</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/1JSCfr9YFx7SAP8sAYS5vx'}</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/1JSCfr9YFx7SAP8sAYS5vx</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>1JSCfr9YFx7SAP8sAYS5vx</t>
+        </is>
+      </c>
+      <c r="G28" t="b">
+        <v>1</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Crazy In Love (Remix)</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>2015-09-04</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K28" t="n">
+        <v>1</v>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>spotify:album:1JSCfr9YFx7SAP8sAYS5vx</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/5a4p39DFm8MN9jhrGxGmU0'}</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/5a4p39DFm8MN9jhrGxGmU0</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>5a4p39DFm8MN9jhrGxGmU0</t>
+        </is>
+      </c>
+      <c r="G29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Pretty Hurts</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>2014-06-17</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K29" t="n">
+        <v>1</v>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>spotify:album:5a4p39DFm8MN9jhrGxGmU0</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/1hq4Vrcbua3DDBLhuWFEVQ'}</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/1hq4Vrcbua3DDBLhuWFEVQ</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>1hq4Vrcbua3DDBLhuWFEVQ</t>
+        </is>
+      </c>
+      <c r="G30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Partition</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>2014-03-18</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K30" t="n">
+        <v>1</v>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>spotify:album:1hq4Vrcbua3DDBLhuWFEVQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/2noKUZhXwUhPQMgSr56T4G'}</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/2noKUZhXwUhPQMgSr56T4G</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>2noKUZhXwUhPQMgSr56T4G</t>
+        </is>
+      </c>
+      <c r="G31" t="b">
+        <v>1</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>BEYONCÉ</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>2013-12-20</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K31" t="n">
+        <v>2</v>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>spotify:album:2noKUZhXwUhPQMgSr56T4G</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/7vZizzCMyhrVSDe7ngA7i8'}</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/7vZizzCMyhrVSDe7ngA7i8</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>7vZizzCMyhrVSDe7ngA7i8</t>
+        </is>
+      </c>
+      <c r="G32" t="b">
+        <v>1</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>4: The Remix</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>2012-04-23</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K32" t="n">
+        <v>6</v>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>spotify:album:7vZizzCMyhrVSDe7ngA7i8</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/73wpHTLtL517aZQleP2zIi'}</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/73wpHTLtL517aZQleP2zIi</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>73wpHTLtL517aZQleP2zIi</t>
+        </is>
+      </c>
+      <c r="G33" t="b">
+        <v>1</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Party (feat. J. Cole)</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>2011-10-24</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K33" t="n">
+        <v>1</v>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>spotify:album:73wpHTLtL517aZQleP2zIi</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/463TYrk70CKqd4eYWhFEDc'}</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/463TYrk70CKqd4eYWhFEDc</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>463TYrk70CKqd4eYWhFEDc</t>
+        </is>
+      </c>
+      <c r="G34" t="b">
+        <v>1</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Run The World (Girls)</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>2011-09-02</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K34" t="n">
+        <v>3</v>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>spotify:album:463TYrk70CKqd4eYWhFEDc</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/34A3G6xkcuxPEuPXZFg44M'}</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/34A3G6xkcuxPEuPXZFg44M</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>34A3G6xkcuxPEuPXZFg44M</t>
+        </is>
+      </c>
+      <c r="G35" t="b">
+        <v>1</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>Best Thing I Never Had</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>2011-09-02</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K35" t="n">
+        <v>4</v>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>spotify:album:34A3G6xkcuxPEuPXZFg44M</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/2mtf43J85iyxUjF57UP1Jl'}</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/2mtf43J85iyxUjF57UP1Jl</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>2mtf43J85iyxUjF57UP1Jl</t>
+        </is>
+      </c>
+      <c r="G36" t="b">
+        <v>1</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>Best Thing I Never Had</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>2011-06-09</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K36" t="n">
+        <v>1</v>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>spotify:album:2mtf43J85iyxUjF57UP1Jl</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/2FpAsisq3cgeeI0ogrxGCG'}</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/2FpAsisq3cgeeI0ogrxGCG</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>2FpAsisq3cgeeI0ogrxGCG</t>
+        </is>
+      </c>
+      <c r="G37" t="b">
+        <v>1</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>Run The World (Girls) - Remixes</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>2011-04-21</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K37" t="n">
+        <v>3</v>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>spotify:album:2FpAsisq3cgeeI0ogrxGCG</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/6sDm2SVKzQaTA2RzQsj3Ev'}</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/6sDm2SVKzQaTA2RzQsj3Ev</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>6sDm2SVKzQaTA2RzQsj3Ev</t>
+        </is>
+      </c>
+      <c r="G38" t="b">
+        <v>1</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>Run The World (Girls)</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>2011-04-21</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K38" t="n">
+        <v>1</v>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>spotify:album:6sDm2SVKzQaTA2RzQsj3Ev</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/10w5joVHMAc9WMfGrQQMmo'}</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/10w5joVHMAc9WMfGrQQMmo</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>10w5joVHMAc9WMfGrQQMmo</t>
+        </is>
+      </c>
+      <c r="G39" t="b">
+        <v>1</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>Fever</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>2010-02-08</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K39" t="n">
+        <v>1</v>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>spotify:album:10w5joVHMAc9WMfGrQQMmo</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/3iClBGMyWVT8hKCL5txMQL'}</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/3iClBGMyWVT8hKCL5txMQL</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>3iClBGMyWVT8hKCL5txMQL</t>
+        </is>
+      </c>
+      <c r="G40" t="b">
+        <v>1</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>Telephone (Tom Neville's Ear Ringer Radio Remix)</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>2010-01-26</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K40" t="n">
+        <v>1</v>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>spotify:album:3iClBGMyWVT8hKCL5txMQL</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/1zAuMqjg441b11Gt4BsUWR'}</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/1zAuMqjg441b11Gt4BsUWR</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>1zAuMqjg441b11Gt4BsUWR</t>
+        </is>
+      </c>
+      <c r="G41" t="b">
+        <v>1</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>Telephone (The Remixes)</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>2010-01-26</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K41" t="n">
+        <v>10</v>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>spotify:album:1zAuMqjg441b11Gt4BsUWR</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/4ZFu2DSRTLXSoRfI0xNvFa'}</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/4ZFu2DSRTLXSoRfI0xNvFa</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>4ZFu2DSRTLXSoRfI0xNvFa</t>
+        </is>
+      </c>
+      <c r="G42" t="b">
+        <v>1</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>Telephone (Ming Extended Remix)</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>2010-01-26</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K42" t="n">
+        <v>1</v>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>spotify:album:4ZFu2DSRTLXSoRfI0xNvFa</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/5XCvVnJoMNOEXrUCC3E5U2'}</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/5XCvVnJoMNOEXrUCC3E5U2</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>5XCvVnJoMNOEXrUCC3E5U2</t>
+        </is>
+      </c>
+      <c r="G43" t="b">
+        <v>1</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>Telephone (Kaskade Extended Remix)</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>2010-01-26</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K43" t="n">
+        <v>1</v>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>spotify:album:5XCvVnJoMNOEXrUCC3E5U2</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/3ZBv9rFQzevDkpbjCj0mCm'}</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/3ZBv9rFQzevDkpbjCj0mCm</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>3ZBv9rFQzevDkpbjCj0mCm</t>
+        </is>
+      </c>
+      <c r="G44" t="b">
+        <v>1</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>Telephone (Electrolightz Remix)</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>2010-01-26</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K44" t="n">
+        <v>1</v>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>spotify:album:3ZBv9rFQzevDkpbjCj0mCm</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/1jq07HQVkXwuIrsVKYLNNT'}</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/1jq07HQVkXwuIrsVKYLNNT</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>1jq07HQVkXwuIrsVKYLNNT</t>
+        </is>
+      </c>
+      <c r="G45" t="b">
+        <v>1</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>Telephone (DJ Dan Extended Vocal Remix)</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>2010-01-26</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K45" t="n">
+        <v>1</v>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>spotify:album:1jq07HQVkXwuIrsVKYLNNT</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/5ZVdq9lpdgszs9Xv5JprsV'}</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/5ZVdq9lpdgszs9Xv5JprsV</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>5ZVdq9lpdgszs9Xv5JprsV</t>
+        </is>
+      </c>
+      <c r="G46" t="b">
+        <v>1</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>Telephone (Crookers Vocal Remix)</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>2010-01-26</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K46" t="n">
+        <v>1</v>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>spotify:album:5ZVdq9lpdgszs9Xv5JprsV</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/5XpL8H1LS4VLYgXAF4DKML'}</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/5XpL8H1LS4VLYgXAF4DKML</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>5XpL8H1LS4VLYgXAF4DKML</t>
+        </is>
+      </c>
+      <c r="G47" t="b">
+        <v>1</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>Telephone (Alphabeat Extended Remix)</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>2010-01-26</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K47" t="n">
+        <v>1</v>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>spotify:album:5XpL8H1LS4VLYgXAF4DKML</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/2a2cEPrFvkzo82xTaHOedw'}</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/2a2cEPrFvkzo82xTaHOedw</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>2a2cEPrFvkzo82xTaHOedw</t>
+        </is>
+      </c>
+      <c r="G48" t="b">
+        <v>1</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>Video Phone</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>2009-11-20</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K48" t="n">
+        <v>3</v>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>spotify:album:2a2cEPrFvkzo82xTaHOedw</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/1wuC0jj7341uFOuCyqzwe8'}</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/1wuC0jj7341uFOuCyqzwe8</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>1wuC0jj7341uFOuCyqzwe8</t>
+        </is>
+      </c>
+      <c r="G49" t="b">
+        <v>1</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>I AM...SASHA FIERCE THE BONUS TRACKS</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>2009-11-20</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K49" t="n">
+        <v>3</v>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>spotify:album:1wuC0jj7341uFOuCyqzwe8</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/0buzXAn3IaIXLK8VjBL6c3'}</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/0buzXAn3IaIXLK8VjBL6c3</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>0buzXAn3IaIXLK8VjBL6c3</t>
+        </is>
+      </c>
+      <c r="G50" t="b">
+        <v>1</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>Broken-Hearted Girl</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>2009-11-20</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K50" t="n">
+        <v>3</v>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>spotify:album:0buzXAn3IaIXLK8VjBL6c3</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>{'spotify': 'https://open.spotify.com/album/3VlJsaBR8fj9Gylfko5I6i'}</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>https://api.spotify.com/v1/albums/3VlJsaBR8fj9Gylfko5I6i</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>3VlJsaBR8fj9Gylfko5I6i</t>
+        </is>
+      </c>
+      <c r="G51" t="b">
+        <v>1</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>Broken-Hearted Girl</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>2009-10-30</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="K51" t="n">
+        <v>2</v>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>album</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>spotify:album:3VlJsaBR8fj9Gylfko5I6i</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: implementação do coletor
</commit_message>
<xml_diff>
--- a/arquivos/coleta_dados_spotify.xlsx
+++ b/arquivos/coleta_dados_spotify.xlsx
@@ -3674,7 +3674,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3757,24 +3757,24 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>208014</v>
+        <v>278106</v>
       </c>
       <c r="D2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>{'spotify': 'https://open.spotify.com/track/1MpCaOeUWhox2Fgigbe1cL'}</t>
+          <t>{'spotify': 'https://open.spotify.com/track/4iN55SUsXVSh8Og9EDyg3z'}</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/1MpCaOeUWhox2Fgigbe1cL</t>
+          <t>https://api.spotify.com/v1/tracks/4iN55SUsXVSh8Og9EDyg3z</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>1MpCaOeUWhox2Fgigbe1cL</t>
+          <t>4iN55SUsXVSh8Og9EDyg3z</t>
         </is>
       </c>
       <c r="H2" t="b">
@@ -3785,12 +3785,12 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>I'M THAT GIRL</t>
+          <t>Broken-Hearted Girl</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>https://p.scdn.co/mp3-preview/efe429b75c7ee5b333e8852b3be22d359778f1ee?cid=19222f3ec658437489e9280a521db7ad</t>
+          <t>https://p.scdn.co/mp3-preview/348979c238d82d9faad82ae8064810e2065dae3c?cid=19222f3ec658437489e9280a521db7ad</t>
         </is>
       </c>
       <c r="L2" t="n">
@@ -3803,7 +3803,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>spotify:track:1MpCaOeUWhox2Fgigbe1cL</t>
+          <t>spotify:track:4iN55SUsXVSh8Og9EDyg3z</t>
         </is>
       </c>
     </row>
@@ -3815,24 +3815,24 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>210372</v>
+        <v>209240</v>
       </c>
       <c r="D3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>{'spotify': 'https://open.spotify.com/track/0mKGwFMHzTprtS2vpR3b6s'}</t>
+          <t>{'spotify': 'https://open.spotify.com/track/6HtFcQNBIjzOZeNJ0IXKDB'}</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/0mKGwFMHzTprtS2vpR3b6s</t>
+          <t>https://api.spotify.com/v1/tracks/6HtFcQNBIjzOZeNJ0IXKDB</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>0mKGwFMHzTprtS2vpR3b6s</t>
+          <t>6HtFcQNBIjzOZeNJ0IXKDB</t>
         </is>
       </c>
       <c r="H3" t="b">
@@ -3843,12 +3843,12 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>COZY</t>
+          <t>Broken-Hearted Girl - Alan Braxe Remix - Radio Edit</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>https://p.scdn.co/mp3-preview/3f4bcb6aa0f4ca5ec1c16525fc530315c5a34652?cid=19222f3ec658437489e9280a521db7ad</t>
+          <t>https://p.scdn.co/mp3-preview/788fc83010024e5d2a2405dc2c87c4a3822536c8?cid=19222f3ec658437489e9280a521db7ad</t>
         </is>
       </c>
       <c r="L3" t="n">
@@ -3861,819 +3861,7 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>spotify:track:0mKGwFMHzTprtS2vpR3b6s</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" t="n">
-        <v>215459</v>
-      </c>
-      <c r="D4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>{'spotify': 'https://open.spotify.com/track/1Hohk6AufHZOrrhMXZppax'}</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>https://api.spotify.com/v1/tracks/1Hohk6AufHZOrrhMXZppax</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>1Hohk6AufHZOrrhMXZppax</t>
-        </is>
-      </c>
-      <c r="H4" t="b">
-        <v>0</v>
-      </c>
-      <c r="I4" t="b">
-        <v>1</v>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>ALIEN SUPERSTAR</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>https://p.scdn.co/mp3-preview/a5715e753ed35f47ec45920a54448b3b109bb39b?cid=19222f3ec658437489e9280a521db7ad</t>
-        </is>
-      </c>
-      <c r="L4" t="n">
-        <v>3</v>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>track</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>spotify:track:1Hohk6AufHZOrrhMXZppax</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" t="n">
-        <v>225388</v>
-      </c>
-      <c r="D5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>{'spotify': 'https://open.spotify.com/track/1xzi1Jcr7mEi9K2RfzLOqS'}</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>https://api.spotify.com/v1/tracks/1xzi1Jcr7mEi9K2RfzLOqS</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>1xzi1Jcr7mEi9K2RfzLOqS</t>
-        </is>
-      </c>
-      <c r="H5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>CUFF IT</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>https://p.scdn.co/mp3-preview/1799de9ff42644af9773b6353358e54615696f19?cid=19222f3ec658437489e9280a521db7ad</t>
-        </is>
-      </c>
-      <c r="L5" t="n">
-        <v>4</v>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>track</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>spotify:track:1xzi1Jcr7mEi9K2RfzLOqS</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" t="n">
-        <v>116727</v>
-      </c>
-      <c r="D6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>{'spotify': 'https://open.spotify.com/track/0314PeD1sQNonfVWix3B2K'}</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>https://api.spotify.com/v1/tracks/0314PeD1sQNonfVWix3B2K</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>0314PeD1sQNonfVWix3B2K</t>
-        </is>
-      </c>
-      <c r="H6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I6" t="b">
-        <v>1</v>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>ENERGY (feat. Beam)</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>https://p.scdn.co/mp3-preview/3b0468d27f6d0c84113fdd973115fdea301109d0?cid=19222f3ec658437489e9280a521db7ad</t>
-        </is>
-      </c>
-      <c r="L6" t="n">
-        <v>5</v>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>track</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>spotify:track:0314PeD1sQNonfVWix3B2K</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" t="n">
-        <v>278281</v>
-      </c>
-      <c r="D7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>{'spotify': 'https://open.spotify.com/track/5pyoxDZ1PX0KxBxiRVxA4U'}</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>https://api.spotify.com/v1/tracks/5pyoxDZ1PX0KxBxiRVxA4U</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>5pyoxDZ1PX0KxBxiRVxA4U</t>
-        </is>
-      </c>
-      <c r="H7" t="b">
-        <v>0</v>
-      </c>
-      <c r="I7" t="b">
-        <v>1</v>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>BREAK MY SOUL</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>https://p.scdn.co/mp3-preview/6277963cb556a9d4d90517197112d732a5fc3b05?cid=19222f3ec658437489e9280a521db7ad</t>
-        </is>
-      </c>
-      <c r="L7" t="n">
-        <v>6</v>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>track</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>spotify:track:5pyoxDZ1PX0KxBxiRVxA4U</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" t="n">
-        <v>224472</v>
-      </c>
-      <c r="D8" t="b">
-        <v>1</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>{'spotify': 'https://open.spotify.com/track/2mqTtvbKxH7SoEQ2oGAnsA'}</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>https://api.spotify.com/v1/tracks/2mqTtvbKxH7SoEQ2oGAnsA</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>2mqTtvbKxH7SoEQ2oGAnsA</t>
-        </is>
-      </c>
-      <c r="H8" t="b">
-        <v>0</v>
-      </c>
-      <c r="I8" t="b">
-        <v>1</v>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>CHURCH GIRL</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>https://p.scdn.co/mp3-preview/aef34f3346148728ab1440b8ba5861bebec9a283?cid=19222f3ec658437489e9280a521db7ad</t>
-        </is>
-      </c>
-      <c r="L8" t="n">
-        <v>7</v>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>track</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>spotify:track:2mqTtvbKxH7SoEQ2oGAnsA</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" t="n">
-        <v>254319</v>
-      </c>
-      <c r="D9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>{'spotify': 'https://open.spotify.com/track/6ufcuVInt0ocHrUimDjGlb'}</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>https://api.spotify.com/v1/tracks/6ufcuVInt0ocHrUimDjGlb</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>6ufcuVInt0ocHrUimDjGlb</t>
-        </is>
-      </c>
-      <c r="H9" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" t="b">
-        <v>1</v>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>PLASTIC OFF THE SOFA</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>https://p.scdn.co/mp3-preview/8e2725101e48c5c3c9b9a79280e8cfe337783b99?cid=19222f3ec658437489e9280a521db7ad</t>
-        </is>
-      </c>
-      <c r="L9" t="n">
-        <v>8</v>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>track</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>spotify:track:6ufcuVInt0ocHrUimDjGlb</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" t="n">
-        <v>368758</v>
-      </c>
-      <c r="D10" t="b">
-        <v>1</v>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>{'spotify': 'https://open.spotify.com/track/0Fl4eWzVaMUOdXcOrj6F1q'}</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>https://api.spotify.com/v1/tracks/0Fl4eWzVaMUOdXcOrj6F1q</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>0Fl4eWzVaMUOdXcOrj6F1q</t>
-        </is>
-      </c>
-      <c r="H10" t="b">
-        <v>0</v>
-      </c>
-      <c r="I10" t="b">
-        <v>1</v>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>VIRGO'S GROOVE</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>https://p.scdn.co/mp3-preview/ae4ae52e313377f6dd438dbf52162a2cb9aad809?cid=19222f3ec658437489e9280a521db7ad</t>
-        </is>
-      </c>
-      <c r="L10" t="n">
-        <v>9</v>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>track</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>spotify:track:0Fl4eWzVaMUOdXcOrj6F1q</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" t="n">
-        <v>203383</v>
-      </c>
-      <c r="D11" t="b">
-        <v>0</v>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>{'spotify': 'https://open.spotify.com/track/5YLGlPYkZBDXieMwzVve7g'}</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>https://api.spotify.com/v1/tracks/5YLGlPYkZBDXieMwzVve7g</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>5YLGlPYkZBDXieMwzVve7g</t>
-        </is>
-      </c>
-      <c r="H11" t="b">
-        <v>0</v>
-      </c>
-      <c r="I11" t="b">
-        <v>1</v>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>MOVE (feat. Grace Jones &amp; Tems)</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>https://p.scdn.co/mp3-preview/883928e4bfbdf64e7ef88497c7381c3d1f54ec58?cid=19222f3ec658437489e9280a521db7ad</t>
-        </is>
-      </c>
-      <c r="L11" t="n">
-        <v>10</v>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>track</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>spotify:track:5YLGlPYkZBDXieMwzVve7g</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="n">
-        <v>1</v>
-      </c>
-      <c r="C12" t="n">
-        <v>260769</v>
-      </c>
-      <c r="D12" t="b">
-        <v>1</v>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>{'spotify': 'https://open.spotify.com/track/1w7cgGZR86yWz1pA2puVJD'}</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>https://api.spotify.com/v1/tracks/1w7cgGZR86yWz1pA2puVJD</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>1w7cgGZR86yWz1pA2puVJD</t>
-        </is>
-      </c>
-      <c r="H12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I12" t="b">
-        <v>1</v>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>HEATED</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>https://p.scdn.co/mp3-preview/98514f25132bcc5c9bcd7bd0d140f6258bd24138?cid=19222f3ec658437489e9280a521db7ad</t>
-        </is>
-      </c>
-      <c r="L12" t="n">
-        <v>11</v>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>track</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>spotify:track:1w7cgGZR86yWz1pA2puVJD</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="n">
-        <v>1</v>
-      </c>
-      <c r="C13" t="n">
-        <v>244792</v>
-      </c>
-      <c r="D13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>{'spotify': 'https://open.spotify.com/track/1LCm0lFnEsxR2oPqyHLGX9'}</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>https://api.spotify.com/v1/tracks/1LCm0lFnEsxR2oPqyHLGX9</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>1LCm0lFnEsxR2oPqyHLGX9</t>
-        </is>
-      </c>
-      <c r="H13" t="b">
-        <v>0</v>
-      </c>
-      <c r="I13" t="b">
-        <v>1</v>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>THIQUE</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>https://p.scdn.co/mp3-preview/6354b49c7a0d9278a17b02e5fbff1ae21f2438bb?cid=19222f3ec658437489e9280a521db7ad</t>
-        </is>
-      </c>
-      <c r="L13" t="n">
-        <v>12</v>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>track</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>spotify:track:1LCm0lFnEsxR2oPqyHLGX9</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="n">
-        <v>1</v>
-      </c>
-      <c r="C14" t="n">
-        <v>169819</v>
-      </c>
-      <c r="D14" t="b">
-        <v>1</v>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>{'spotify': 'https://open.spotify.com/track/3k4CoiIQXiNBrwrmbBMDxj'}</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>https://api.spotify.com/v1/tracks/3k4CoiIQXiNBrwrmbBMDxj</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>3k4CoiIQXiNBrwrmbBMDxj</t>
-        </is>
-      </c>
-      <c r="H14" t="b">
-        <v>0</v>
-      </c>
-      <c r="I14" t="b">
-        <v>1</v>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>ALL UP IN YOUR MIND</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>https://p.scdn.co/mp3-preview/01548e43349e0d6e08423de7eded6c3f86b2b133?cid=19222f3ec658437489e9280a521db7ad</t>
-        </is>
-      </c>
-      <c r="L14" t="n">
-        <v>13</v>
-      </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>track</t>
-        </is>
-      </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>spotify:track:3k4CoiIQXiNBrwrmbBMDxj</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" t="n">
-        <v>1</v>
-      </c>
-      <c r="C15" t="n">
-        <v>198897</v>
-      </c>
-      <c r="D15" t="b">
-        <v>1</v>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>{'spotify': 'https://open.spotify.com/track/2XMAWynSTIst5KmLSv0Npf'}</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>https://api.spotify.com/v1/tracks/2XMAWynSTIst5KmLSv0Npf</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>2XMAWynSTIst5KmLSv0Npf</t>
-        </is>
-      </c>
-      <c r="H15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I15" t="b">
-        <v>1</v>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>AMERICA HAS A PROBLEM</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>https://p.scdn.co/mp3-preview/5251e13693f98f53cad47b2ef2a3b9c0b188fb5f?cid=19222f3ec658437489e9280a521db7ad</t>
-        </is>
-      </c>
-      <c r="L15" t="n">
-        <v>14</v>
-      </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>track</t>
-        </is>
-      </c>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>spotify:track:2XMAWynSTIst5KmLSv0Npf</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" t="n">
-        <v>1</v>
-      </c>
-      <c r="C16" t="n">
-        <v>288254</v>
-      </c>
-      <c r="D16" t="b">
-        <v>1</v>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>{'spotify': 'https://open.spotify.com/track/4DByEumlGTZKSzuVEZ35eo'}</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>https://api.spotify.com/v1/tracks/4DByEumlGTZKSzuVEZ35eo</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>4DByEumlGTZKSzuVEZ35eo</t>
-        </is>
-      </c>
-      <c r="H16" t="b">
-        <v>0</v>
-      </c>
-      <c r="I16" t="b">
-        <v>1</v>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>PURE/HONEY</t>
-        </is>
-      </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>https://p.scdn.co/mp3-preview/a4564eeac7ee46de87873d6e77cff980e8bc4b58?cid=19222f3ec658437489e9280a521db7ad</t>
-        </is>
-      </c>
-      <c r="L16" t="n">
-        <v>15</v>
-      </c>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t>track</t>
-        </is>
-      </c>
-      <c r="N16" t="inlineStr">
-        <is>
-          <t>spotify:track:4DByEumlGTZKSzuVEZ35eo</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="n">
-        <v>1</v>
-      </c>
-      <c r="C17" t="n">
-        <v>273997</v>
-      </c>
-      <c r="D17" t="b">
-        <v>1</v>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>{'spotify': 'https://open.spotify.com/track/3HyR1j49TY5ACP2lseF1jx'}</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>https://api.spotify.com/v1/tracks/3HyR1j49TY5ACP2lseF1jx</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>3HyR1j49TY5ACP2lseF1jx</t>
-        </is>
-      </c>
-      <c r="H17" t="b">
-        <v>0</v>
-      </c>
-      <c r="I17" t="b">
-        <v>1</v>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>SUMMER RENAISSANCE</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>https://p.scdn.co/mp3-preview/b8ae9f9e20dd574130d6bcedb63c2c60e4c2ae08?cid=19222f3ec658437489e9280a521db7ad</t>
-        </is>
-      </c>
-      <c r="L17" t="n">
-        <v>16</v>
-      </c>
-      <c r="M17" t="inlineStr">
-        <is>
-          <t>track</t>
-        </is>
-      </c>
-      <c r="N17" t="inlineStr">
-        <is>
-          <t>spotify:track:3HyR1j49TY5ACP2lseF1jx</t>
+          <t>spotify:track:6HtFcQNBIjzOZeNJ0IXKDB</t>
         </is>
       </c>
     </row>
@@ -4688,7 +3876,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4754,12 +3942,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>spotify:track:1w7cgGZR86yWz1pA2puVJD</t>
+          <t>spotify:track:6HtFcQNBIjzOZeNJ0IXKDB</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>HEATED</t>
+          <t>Broken-Hearted Girl - Alan Braxe Remix - Radio Edit</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -4769,26 +3957,26 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>spotify:artist:6vWDO969PvNqNYHIOW5v0m</t>
+          <t>spotify:artist:24JRvbKfTcF2x7c2kCCJrW</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Beyoncé</t>
+          <t>Alan Braxe</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://i.scdn.co/image/ab677762000078e645c984e8c82f9ce15ebf1f51</t>
+          <t>https://i.scdn.co/image/ab677762000078e6aae517f57fa4e9833b4bce9c</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>['main artist']</t>
+          <t>['remixer']</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>0.8999000191688538</v>
+        <v>0.7479000091552734</v>
       </c>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
@@ -4799,44 +3987,44 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>spotify:track:1w7cgGZR86yWz1pA2puVJD</t>
+          <t>spotify:track:6HtFcQNBIjzOZeNJ0IXKDB</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>HEATED</t>
+          <t>Broken-Hearted Girl - Alan Braxe Remix - Radio Edit</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Writers</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
+          <t>Performers</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>spotify:artist:6vWDO969PvNqNYHIOW5v0m</t>
+        </is>
+      </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Brittany "@Chi_Coney" Coney</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr"/>
+          <t>Beyoncé</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>https://i.scdn.co/image/ab677762000078e645c984e8c82f9ce15ebf1f51</t>
+        </is>
+      </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['main artist']</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>https://artists.spotify.com/songwriter/1uYXu9L0vzo1lcJk7SjgCT</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>spotify:songwriter:1uYXu9L0vzo1lcJk7SjgCT</t>
-        </is>
-      </c>
+        <v>0.8999000191688538</v>
+      </c>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -4844,12 +4032,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>spotify:track:1w7cgGZR86yWz1pA2puVJD</t>
+          <t>spotify:track:6HtFcQNBIjzOZeNJ0IXKDB</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>HEATED</t>
+          <t>Broken-Hearted Girl - Alan Braxe Remix - Radio Edit</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -4857,44 +4045,44 @@
           <t>Writers</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>spotify:artist:3aVoqlJOYx31lH1gibGDt3</t>
+        </is>
+      </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Denisia "Blu June" Andrews</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr"/>
+          <t>Babyface</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>https://i.scdn.co/image/ab677762000078e6d2b377637d9f6ed34f1652e2</t>
+        </is>
+      </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['composer', 'lyricist']</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>https://artists.spotify.com/songwriter/6usZxRd8e7TQwcksnohR1U</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>spotify:songwriter:6usZxRd8e7TQwcksnohR1U</t>
-        </is>
-      </c>
+        <v>0.6998000144958496</v>
+      </c>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>spotify:track:1w7cgGZR86yWz1pA2puVJD</t>
+          <t>spotify:track:6HtFcQNBIjzOZeNJ0IXKDB</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>HEATED</t>
+          <t>Broken-Hearted Girl - Alan Braxe Remix - Radio Edit</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -4902,51 +4090,59 @@
           <t>Writers</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>spotify:artist:59mvY7ziUSNoyIGgErHemV</t>
+        </is>
+      </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>A. Graham</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr"/>
+          <t>Mikkel Storleer Eriksen</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>https://i.scdn.co/image/ab677762000078e6afc079cda32d54850e82c385</t>
+        </is>
+      </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['composer', 'lyricist']</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>0.6995999813079834</v>
       </c>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>spotify:track:1w7cgGZR86yWz1pA2puVJD</t>
+          <t>spotify:track:6HtFcQNBIjzOZeNJ0IXKDB</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>HEATED</t>
+          <t>Broken-Hearted Girl - Alan Braxe Remix - Radio Edit</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Producers</t>
+          <t>Writers</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>spotify:artist:2pSxft78wxISNLTbjFThTk</t>
+          <t>spotify:artist:7BwWmXxaUFHTL8f8IeszOZ</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Cadenza</t>
+          <t>Tor Erik Hermansen</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -4956,27 +4152,27 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>['producer']</t>
+          <t>['composer', 'lyricist']</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>0.548799991607666</v>
+        <v>0.6988999843597412</v>
       </c>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>spotify:track:1w7cgGZR86yWz1pA2puVJD</t>
+          <t>spotify:track:6HtFcQNBIjzOZeNJ0IXKDB</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>HEATED</t>
+          <t>Broken-Hearted Girl - Alan Braxe Remix - Radio Edit</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -4986,17 +4182,17 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>spotify:artist:6PIl48ctj6HDmqVM2uIikd</t>
+          <t>spotify:artist:0rwyRIAM4qMPtYvkC0pECf</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Kelman Duran</t>
+          <t>StarGate for 45th &amp; 3rd Music LLC</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>https://i.scdn.co/image/ab677762000078e645c984e8c82f9ce15ebf1f51</t>
+          <t>https://i.scdn.co/image/ab677762000078e6aae517f57fa4e9833b4bce9c</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -5005,23 +4201,23 @@
         </is>
       </c>
       <c r="I7" t="n">
-        <v>0.5483999848365784</v>
+        <v>0.5491999983787537</v>
       </c>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>spotify:track:1w7cgGZR86yWz1pA2puVJD</t>
+          <t>spotify:track:6HtFcQNBIjzOZeNJ0IXKDB</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>HEATED</t>
+          <t>Broken-Hearted Girl - Alan Braxe Remix - Radio Edit</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -5031,17 +4227,17 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>spotify:artist:7rzPhcWW1k8njDS5r2xbWe</t>
+          <t>spotify:artist:0GAqvwpLwRPnWjy5TJKfoT</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Jahaan Sweet</t>
+          <t>Beyoncé Knowles for Music World Music, LLC</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>https://i.scdn.co/image/ab677762000078e6afc079cda32d54850e82c385</t>
+          <t>https://i.scdn.co/image/ab677762000078e6aae517f57fa4e9833b4bce9c</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -5050,235 +4246,10 @@
         </is>
       </c>
       <c r="I8" t="n">
-        <v>0.5480999946594238</v>
+        <v>0.5490000247955322</v>
       </c>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>spotify:track:1w7cgGZR86yWz1pA2puVJD</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>HEATED</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Producers</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>spotify:artist:2TRy6nJhEnznYDL0AtYJAI</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Stuart White</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>https://i.scdn.co/image/ab677762000078e6d2b377637d9f6ed34f1652e2</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>['producer']</t>
-        </is>
-      </c>
-      <c r="I9" t="n">
-        <v>0.5473999977111816</v>
-      </c>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>spotify:track:1w7cgGZR86yWz1pA2puVJD</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>HEATED</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Producers</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>spotify:artist:0NPWbgGDaiX1yZaN0nzhqn</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Neenyo</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>https://i.scdn.co/image/ab677762000078e6d2b377637d9f6ed34f1652e2</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>['producer']</t>
-        </is>
-      </c>
-      <c r="I10" t="n">
-        <v>0.5472000241279602</v>
-      </c>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>spotify:track:1w7cgGZR86yWz1pA2puVJD</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>HEATED</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Producers</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>spotify:artist:6T9dsSIQ31Sk8x24lwfTG4</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>Sevn Thomas</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>https://i.scdn.co/image/ab677762000078e6d2b377637d9f6ed34f1652e2</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>['producer']</t>
-        </is>
-      </c>
-      <c r="I11" t="n">
-        <v>0.5468999743461609</v>
-      </c>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>spotify:track:1w7cgGZR86yWz1pA2puVJD</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>HEATED</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Producers</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>spotify:artist:2RQnTQM6OQd8dTUDF7UsT7</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>Boi-1da</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>https://i.scdn.co/image/ab677762000078e6aae517f57fa4e9833b4bce9c</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>['producer']</t>
-        </is>
-      </c>
-      <c r="I12" t="n">
-        <v>0.5468000173568726</v>
-      </c>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>spotify:track:1w7cgGZR86yWz1pA2puVJD</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>HEATED</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Producers</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>spotify:artist:3FdxqLD6H5pfO0C0kd9YYt</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>Harry Edwards</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>https://i.scdn.co/image/ab677762000078e645c984e8c82f9ce15ebf1f51</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>['producer']</t>
-        </is>
-      </c>
-      <c r="I13" t="n">
-        <v>0.5461000204086304</v>
-      </c>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>